<commit_message>
can select according time and progress
</commit_message>
<xml_diff>
--- a/新建 Microsoft Excel Worksheet - 副本 (2) - 副本.xlsx
+++ b/新建 Microsoft Excel Worksheet - 副本 (2) - 副本.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
   <si>
     <t>责任人</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,6 +68,14 @@
   </si>
   <si>
     <t>王影</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计划开始时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计划完成时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -111,9 +119,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -447,22 +456,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="2" max="2" width="9" style="1"/>
     <col min="5" max="5" width="13.375" customWidth="1"/>
+    <col min="6" max="6" width="15.625" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
@@ -474,8 +486,14 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -491,8 +509,14 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2" s="2">
+        <v>42399</v>
+      </c>
+      <c r="G2" s="2">
+        <v>42460</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -508,8 +532,14 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3" s="2">
+        <v>42399</v>
+      </c>
+      <c r="G3" s="2">
+        <v>42460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -525,8 +555,14 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4" s="2">
+        <v>42399</v>
+      </c>
+      <c r="G4" s="2">
+        <v>42460</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -542,8 +578,14 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F5" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G5" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -559,8 +601,14 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F6" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G6" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -576,8 +624,14 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F7" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G7" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -593,8 +647,14 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F8" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G8" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -610,8 +670,14 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F9" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G9" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -627,8 +693,14 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F10" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G10" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -644,8 +716,14 @@
       <c r="E11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F11" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G11" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -661,8 +739,14 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F12" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G12" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -678,8 +762,14 @@
       <c r="E13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F13" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G13" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -695,8 +785,14 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F14" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G14" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -712,8 +808,14 @@
       <c r="E15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F15" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G15" s="2">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -728,6 +830,12 @@
       </c>
       <c r="E16" t="s">
         <v>10</v>
+      </c>
+      <c r="F16" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G16" s="2">
+        <v>42734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>